<commit_message>
janya 19 ended at 19860925
</commit_message>
<xml_diff>
--- a/dataset/cleaned csv/cleaned csv.xlsx
+++ b/dataset/cleaned csv/cleaned csv.xlsx
@@ -14,12 +14,390 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Text</t>
   </si>
   <si>
     <t>CASE: A 28-year-old previously healthy man presented with a 6-week history of palpitations. The symptoms occurred during rest, 2–3 times per week, lasted up to 30 minutes at a time and were associated with dyspnea. Except for a grade 2/6 holosystolic tricuspid regurgitation murmur (best heard at the left sternal border with inspiratory accentuation), physical examination yielded unremarkable findings. An electrocardiogram (ECG) revealed normal sinus rhythm and a Wolff– Parkinson– White pre-excitation pattern (Fig.1: Top), produced by a right-sided accessory pathway. Transthoracic echocardiography demonstrated the presence of Ebstein's anomaly of the tricuspid valve, with apical displacement of the valve and formation of an “atrialized” right ventricle (a functional unit between the right atrium and the inlet [inflow] portion of the right ventricle) (Fig.2). The anterior tricuspid valve leaflet was elongated (Fig.2C, arrow), whereas the septal leaflet was rudimentary (Fig.2C, arrowhead). Contrast echocardiography using saline revealed a patent foramen ovale with right-to-left shunting and bubbles in the left atrium (Fig.2D). The patient underwent an electrophysiologic study with mapping of the accessory pathway, followed by radiofrequency ablation (interruption of the pathway using the heat generated by electromagnetic waves at the tip of an ablation catheter). His post-ablation ECG showed a prolonged PR interval and an odd “second” QRS complex in leads III, aVF and V2–V4 (Fig.1Bottom), a consequence of abnormal impulse conduction in the “atrialized” right ventricle. The patient reported no recurrence of palpitations at follow-up 6 months after the ablation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The patient was a 34-yr-old man who presented with complaints of fever and a chronic cough.
+He was a smoker and had a history of pulmonary tuberculosis that had been treated and cured.
+A computed tomographic (CT) scan revealed multiple tiny nodules in both lungs.
+A thoracoscopic lung biopsy was taken from the right upper lobe.
+The microscopic examination revealed a typical LCH.
+The tumor cells had vesicular and grooved nuclei, and they formed small aggregations around the bronchioles (Fig.1).
+The tumor cells were strongly positive for S-100 protein, vimentin, CD68 and CD1a.
+There were infiltrations of lymphocytes and eosinophils around the tumor cells.
+With performing additional radiologic examinations, no other organs were thought to be involved.
+He quit smoking, but he received no other specific treatment.
+He was well for the following one year.
+After this, a follow-up CT scan was performed and it showed a 4 cm-sized mass in the left lower lobe, in addition to the multiple tiny nodules in both lungs (Fig.2).
+A needle biopsy specimen revealed the possibility of a sarcoma; therefore, a lobectomy was performed.
+Grossly, a 4 cm-sized poorly-circumscribed lobulated gray-white mass was found (Fig.3), and there were a few small satellite nodules around the main mass.
+Microscopically, the tumor cells were aggregated in large sheets and they showed an infiltrative growth.
+The cytologic features of some of the tumor cells were similar to those seen in a typical LCH.
+However, many tumor cells showed overtly malignant cytologic features such as pleomorphic/hyperchromatic nuclei and prominent nucleoli (Fig.4), and multinucleated tumor giant cells were also found.
+There were numerous mitotic figures ranging from 30 to 60 per 10 high power fields, and some of them were abnormal.
+A few foci of typical LCH remained around the main tumor mass.
+Immunohistochemically, the tumor cells were strongly positive for S-100 protein (Fig.5) and vimentin; they were also positive for CD68 (Dako N1577, Clone KPI), and focally positive for CD1a (Fig.6), and they were negative for cytokeratin, epithelial membrane antigen, CD3, CD20 and HMB45.
+The ultrastructural analysis failed to demonstrate any Birbeck granules in the cytoplasm of the tumor cells.
+Now, at five months after lobectomy, the patient is doing well with no significant change in the radiologic findings.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 23 year old white male with a 4 year history of Crohn's disease presented with an acute two day history of malaise, fever, abdominal pain, vomiting and stomal diarrhoea.
+He complained of joint pains affecting the shoulders, elbows, wrists, metacarpophalangeals, knees and ankles.
+There was also a rash on the elbows, ankles and feet, which began as erythematous macules and evolved to vesico-pustular lesions followed by crusting.
+There was no history of sexual exposure or any intercurrent infection.
+He was on no regular medication, but had discontinued Pentasa 4 months earlier.
+One month earlier he had undergone a laparotomy to excise a complex ileo-cutaneous fistula with blind tracts, and two weeks earlier a defunctioning ileostomy had been created in view of persistent abdominal pain.
+The cutaneous fistula had been present for a year, but was associated with a terminal ileal stricture and ileo-rectal fistula of at least 2 years duration.
+His bowel disease had been resistant to immunosuppressive drugs including azathioprine, corticosteroiods and three infusions of Infliximab a year earlier.
+There had been no extra-intestinal manifestations.
+On admission to the hospital, he was thin, afebrile with a resting tachycardia of 125/minute.
+The rest of the cardio-respiratory examination was normal.
+The abdomen was minimally tender around the ileostomy without guarding or rebound tenderness.
+Examination of the skin revealed some pustules and crusts around the elbows, ankles and feet (Fig 1 and  2).
+The buttocks were spared.
+There were clinical signs of synovitis of the wrists, proximal interphalangeal and metacarpophalangeal joints, and also both ankles.
+Results of the laboratory tests showed a haemoglobin of 13.1 gm/dl, white blood count 15.8 × 109/L, platelets 585 × 109/L, C- reactive protein 37.7 mg/L and erythrocyte sedimentation rate 69 mm/hr.
+Urea and electrolytes, complement, urine analysis and microscopy were normal.
+Rheumatoid factor, antinuclear and antineutrophil cytoplasmic antibodies, cryoglobulins and Hepatitis B and C serology were negative.
+Transthoracic echocardiogram showed no signs of endocarditis, and multiple blood cultures were sterile.
+A skin biopsy from the ankle revealed a perivascular lymphohistiocytic infiltrate with prominent neutrophils and associated fibrinoid necrosis of vessels consistent with 'leukocytoclastic' vasculitis.
+He was commenced on 60 mg prednisolone per day leading to prompt and complete resolution of all features.
+The dose of prednisolone was rapidly tapered over the course of one month by the patient, faster than advised but without any recurrence over the following 3 years.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 30-year-old female (65 kg) underwent rhinoplasty under general anaesthesia, which was induced using a combination of a bolus of Remifentanyl (0.5 μg/kg) and Propofol 2 mg/kg.
+Muscle paralysis was obtained with Cisatracurium (0.15 μg/kg).
+Transoral intubation was performed with a Macintosh blade (No.3) and a size 7 mm diameter reinforced tracheal tube was easily and gently placed in the trachea, on the first attempt and was then fixed to the right corner of the mouth.
+No problems were encountered during laryngoscopy and intubation.
+The cuff of the tube was inflated with a pressure ≤ 20 cm H2O.
+No adjustment of cuff volume was made intra-operatively.
+N2O was not used for inhalation anaesthesia.
+The throat pack was placed in the pharynx to avoid the passage of blood in the aero-digestive tract.
+General anaesthesia was maintained with Sevofluorane in oxygen/air and Remifentanyl in continuous infusion 0.25 μg/kg/min.
+Moderate arterial hypotension was maintained with a cuff systolic artery pressure of approximately 90 mmHg.
+The operation was carried out in a semi-supine position with the head slightly inclined forward and laterally and trunk slightly elevated.
+Duration of the operation was 100 minutes.
+The patient was extubated, after removal of the throat pack without problems.
+The following day the patient complained of difficulty in swallowing, dysphonia and hoarseness.
+Examination revealed deviation of the tongue to the right side and vocal cord paralysis, expression of hypoglossal and recurrent laryngeal nerve injury without local oedema or haematoma.
+The movements of the pharynx and soft palate were normal.
+Meticulous neurological examination, including also magnetic resonance imaging (MRN) revealed no other evidence of central or cranial nerve involvement.
+Conservative management included steroids, vitamins together with speech and swallowing therapy.
+Full recovery of lingual and laryngeal functions was obtained within four months after surgery.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here, we describe another case in a 60-year-old man from San Francisco who had consumed raw pork while traveling in the Philippines.
+In June 2003, this man became ill with fever, diaphoresis, headache, nausea, and anorexia.
+He had just returned from a 7-month vacation in the Philippines.
+Three days after symptoms onset, his physician prescribed doxycycline.
+Symptoms continued and he was admitted to a local hospital 5 days later with a fever of 38.9°C, nuchal rigidity, headache, and general malaise.
+The patient described no recent contact with sick persons; past medical history was unremarkable.
+On physical examination, he was somnolent but fully oriented, with no focal findings on neurologic examination and only slight nuchal rigidity.
+He had a leukocyte count of 21,000/mm3, including 16,400/mm3 neutrophils.
+Cerebrospinal fluid (CSF) showed leukocyte count of 487/μL with 80% polymorphonuclear cells and 18% lymphocytes, and glucose and protein levels &lt;20 mg/dL and &lt;167 mg/dL, respectively.
+Gram stain of CSF showed gram-positive cocci in pairs (Figure).
+Empiric therapy (ceftriaxone, vancomycin, and ampicillin) for bacterial meningitis was begun.
+Computed tomographic scan of the head showed only sinusitis; findings of chest radiograph and transesophageal echocardiogram were negative.
+On hospital day 2, blood cultures grew gram-positive cocci in pairs and chains.
+The organism was catalase-negative, bile esculin-negative, and pyrrolidonyl aminopeptidase-negative, consistent with Streptococcus spp.
+A latex agglutination test did not detect Streptococcus pneumoniae antigen.
+Antimicrobial susceptibility testing showed that the isolate was sensitive to penicillin (MIC = 0.03), ceftriaxone, and vancomycin but resistant to tetracycline and clindamycin.
+Antimicrobial therapy was changed to penicillin G, 24 million units intravenously per day.
+On hospital day 5, the patient complained of hearing loss in his left ear.
+Results of nasopharyngeal endoscopy were negative.
+By hospital day 7, the organism was identified by the API 20 Strep System (bioMerieux, Marcy l’Etoile, France), as S. suis serotype 2.
+The patient subsequently stated that he was a butcher with a culinary preference for partially cooked pork, which he had eaten in the Philippines until the week prior to onset of symptoms.
+On hospital day 9, a formal audiology evaluation showed severe bilateral sensorineural high-frequency hearing loss (–70 dB).
+The patient completed a 10-day course of parenteral antimicrobial drugs and was discharged on continued oral therapy with close followup.
+Two months after discharge, the patient reported much improved hearing without other sequelae.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 74-year-old man was referred to our hospital in November 2000 because of liver dysfunction detected during a medical checkup.
+The patient had been diagnosed with nephrotic syndrome in 1995.
+Laboratory examinations showed elevated serum hepatobiliary enzymes and IgM, and the presence of antimitochondrial antibodies.
+Serologic markers for Hepatitis B and C viruses were negative.
+Histopathologic examination of a liver biopsy specimen obtained at laparoscopy revealed non-suppurative destructive cholangitis in the portal area (Figure ​1).
+The diagnosis of PBC (Scheuer stage 3) was confirmed and ursodeoxycholic acid, 900 mg daily, was started.
+In January and June 2002, the patient underwent endoscopic variceal ligation plus endoscopic injection sclerotherapy as well as argon plasma coagulation for worsening esophageal varices.
+In September 2007, the patient was admitted for the treatment of recurrent esophageal varices.
+The platelet count had ranged between 52 × 109/L and 69 × 109/L for several years, but it was noted to decrease from 61 × 109/L in June 2007 to 8 × 109/L just before admission.
+Before the deterioration of thrombocytopenia, the patient had no infectious diseases and received no other medication.
+On admission, the patient had neither purpura nor bleeding episodes.
+Table 1 shows the laboratory data on admission.
+The platelet-associated IgG level was markedly high.
+Bone marrow biopsy revealed normocellular marrow without cellular atypia.
+Ultrasonography and magnetic resonance imaging revealed a cirrhotic liver with splenomegaly, ascites, and gallstones.
+The spleen size had remained unchanged from previous imaging examinations.
+Based on these findings, the association of PBC (decompensated liver cirrhosis) with ITP was diagnosed.
+Human leukocyte antigen (HLA) genotyping determined by polymerase chain reaction-sequencing-based typing or polymerase chain reaction-sequence specific primers (SRL, Inc., Tokyo, Japan) detected A*02010101, B*400201, C*030401, C*07020101, DPB1*0501, DQA1*0103, DQA1*030101, DQB1*030201, DQB1*060101, DRB1*080201, and DRB1*080302.
+The 13C urea breath test for H pylori infection was negative.
+Figure ​2 shows the clinical course.
+Oral prednisolone, 30 mg daily, for ITP was started on day 11, and diuretic therapy combined with albumin infusion for ascites was performed.
+As the platelet count did not increase notably, pulse therapy with intravenous methylprednisolone, 1 g daily, was added on d 22 to 24.
+However, the response was weak and temporary.
+On d 31, mild melena was identified.
+The patient was given a trial of intravenous immune gamma globulin therapy, 25 g daily, on d 32 to 36, combined with a second round of intravenous methylprednisolone pulse therapy on d 32 to 34.
+Because a moderate response was observed, prednisolone was continued, and the platelet count increased slowly.
+The ascites was relatively well controlled with diuretics at discharge.
+Considering the decompensated liver cirrhosis and the platelet count, we determined the patient required careful follow-up of esophageal varices without prophylactic endoscopic therapy.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An 18-year-old male was diagnosed with attention-deficit hyperactivity disorder (ADHD) in 2005.
+He was overweight with a body mass index (BMI) of 40.
+He was started on quetiapine fumarate (Seroquel®) 900 mg daily in April 2005 and methylphenidate (Concerta®) 54 mg daily in September 2005.
+In the beginning of August 2006 he was admitted to his local hospital with severe dyspnoea, tachypnea, tachycardia, and cyanosis.
+On admission the blood pressure was 120/80 mmHg, and the arterial blood gas revealed a pH of 7.45, pCO2 of 3.55 kPa, paO2 of 7.76 kPa, and BE of −5.1 mmol/l.
+C-reactive protein was not elevated.
+The chest X-ray showed an enlarged heart.
+He developed hemoptysis and was treated with unfractionated heparin in suspicion of pulmonary embolism.
+He subsequently developed cardiogenic shock and was treated with vasoactive drugs.
+In spite of the treatment he became oliguric and his liver enzymes were rising.
+He was referred to our hospital for further treatment.
+On admission the blood pressure was 90/60 mmHg, despite infusion with noradrenaline.
+His heart rate was 130/minute and his temperature was 38.4 °C.
+A thoracic computed tomography scan did not show pulmonary embolism.
+Echocardiography revealed biventricular failure and left ventricular end diastolic diameter was 7 cm.
+The left ventricle was severely hypokinetic with an ejection fraction (EF) of 20%–25%.
+The left ventricular end diastolic pressure was markedly elevated, and there was a moderate mitral regurgitation.
+Intermittent hemodialysis was initiated.
+His liver function improved slightly, but despite dialysis the renal function deteriorated with increasing creatinine values.
+After three days there was a further worsening of the left ventricular systolic function with an ejection fraction of 10%–12% and marked pulmonary hypertension with systolic pulmonary pressure estimated to 30 mmHg.
+The clinical picture resembled dilated cardiomyopathy with low output failure causing renal and liver failure.
+We suspected drug-induced cardiomyopathy and methylphenidate and quetiapine fumarate were discontinued.
+Screening for infectious pathogens, immunological markers, and iron or amyloid deposition were all negative.
+After three days he was transferred to the National Hospital (Rikshospitalet, Oslo) with ongoing noradrenaline and dobutamine infusions.
+Shortly after admission an intraaortic balloon pump (IABP) was inserted and noradrenaline was replaced by nitroprusside.
+Coronary angiography was normal.
+Endomyocardial biopsy from the right ventricle did not reveal any distinct myocardial pathology.
+On treatment with IABP, nitroprusside, and dialysis, the clinical situation gradually improved and the liver function returned to normal.
+His renal function also improved with increasing diuresis and creatinine fell from 798 to 98 μmol/l.
+His EF was still markedly reduced (15%).
+Because of behavioral problems and adipose stature, he was denied a heart transplant.
+He was treated with IABP for 26 days, and after 28 days he was transferred back to our hospital.
+At that time his liver and renal functions were normal.
+He was treated with an angiotensin-converting enzyme (ACE)-inhibitor, a beta-blocker, and diuretics.
+During the following two weeks his clinical status improved and he was subsequently discharged to his home.
+The echocardiography still showed markedly dilated left ventricle with EF of 20%.
+In March 2007, his clinical status was improved and he was in function class II (New York Heart Association) with an EF estimated by echocardiography to 30%–35%.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 19-year-old man presented at the emergency department, 12 h after insertion of a high pressure container with tanning spray into his rectum.
+A plain abdominal radiograph (Figure 1) showed the container in the rectosigmoid region.
+There were no signs of perforation.
+A flexible sigmoidoscopy was performed under conscious sedation.
+The object was located just above the rectosigmoid junction.
+The container could not be extracted by bimanual manipulation.
+An attempt to remove the object with conventional endoscopic instruments, such as polypectomy snares, was unsuccessful.
+The sigmoidoscope could be passed alongside the foreign body to its proximal end.
+A guide wire was left behind with the sigmoidoscope removed.
+Subsequently, a 40 mm pneumatic dilatation balloon (Rigiflex®, Boston Scientific), normally used in achalasia patients, was inserted over the guide wire and inflated just above the container (Figure 2).
+For safety purposes, the sigmoidoscope was reintroduced alongside the catheter of the balloon to allow endoscopic visual control of the distal end of the container in the rectum.
+Gentle traction was exerted on the balloon catheter, and the container was successfully removed under fluoroscopic and endoscopic control (Figure ​3).
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 63-year-old woman with no known cardiac history presented with a sudden onset of dyspnea requiring intubation and ventilatory support out of hospital.
+She denied preceding symptoms of chest discomfort, palpitations, syncope or infection.
+The patient was afebrile and normotensive, with a sinus tachycardia of 140 beats/min.
+The cardiorespiratory examination was remarkable for an elevated jugular venous pressure at the angle of the jaw, a left-sided third heart sound and bibasilar crackles in both lung fields.
+The complete blood cell count, electrolytes and cardiac biomarkers were within normal limits.
+An initial electrocardiogram revealed ST depression in leads V2 to V6, suggestive of anterolateral ischemia (Figure 1).
+A chest radiograph demonstrated pulmonary vascular congestion consistent with a diagnosis of pulmonary edema (Figure 2).
+An echocardiographic examination revealed normal cardiac dimensions, normal wall motion and mild diastolic dysfunction with an early diastolic to late diastolic transmitral ratio of less than 1, prolonged deceleration time (250 ms) and a reduced early diastolic annular velocity of the lateral mitral valve annulus.
+Following aggressive diuresis and requiring minimal ventilatory support, the patient was extubated one day following her initial presentation.
+Within 1 h of extubation, the patient developed recurrent pulmonary edema clinically and radiographically, requiring mechanical ventilation.
+Cardiac catheterization was performed and revealed normal coronary arteries.
+On day 4 of the coronary care unit admission, the patient failed a repeat attempt at extubation.
+A computed tomographic scan revealed a 4 cm × 9 cm multinodular goiter extending into the mediastinum and suspected associated tracheal stenosis (Figure 3).
+With a diagnosis of NPPE secondary to an enlarged goiter, the patient underwent surgical intervention for a thyroidectomy.
+Intraoperative bronchoscopy revealed tracheal stenosis of greater than 50%.
+The postoperative course was uncomplicated, and three months following discharge, the patient returned to her previous activity level without subjective dyspnea.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 28-year-old woman was referred with a 4-week history of continuous, moderate right upper quadrant pain associated with jaundice, as well as weight loss (10 kg over 3 months) and a liver mass identified by ultrasonography.
+The pain sensation seemed different from previous colicky attacks the patient had experienced before she underwent laparoscopic cholecystectomy 7 years previously.
+On physical examination, she was obese (body mass index 37.8), with icterus noted over the conjunctivae, oral mucosa and skin.
+Imaging modalities included computed tomography (CT), positron emission tomography (PET) and endoscopic cholangiopancreatography (ERCP) (Fig.1).
+The patient underwent exploratory laparotomy.
+Intraoperative ultrasonography revealed a cystic lesion measuring 3.5 2.5 cm within the central portion of the liver, anterior to the porta hepatis.
+Intraoperative cholangiography demonstrated an extensive stricture obliterating the left hepatic duct, with partial occlusion of the right hepatic duct.
+An extended left lobectomy was done en bloc with the biliary confluence.
+On frozen-section examination, all margins of the excised specimen were free of malignant cells.
+Reconstruction was performed with a Roux-en-Y cholangiojejunostomy to 3 second bile duct radicals in the right side.
+Intraoperatively, radiotherapy was applied to the surgical margins.
+After this, the patient underwent 6 weeks of image-guided external beam radiation centred on the resection field labelled at surgery.
+The final pathology described this tumour as an infiltrating, moderately differentiated squamous cell carcinoma associated with severe dysplasia of the bile-duct epithelium (Fig.2).
+The patient recovered without complications and was doing well 18 months after the initial surgical procedure, with an unremarkable CT scan.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 49-year-old woman was admitted to the Department of Radiology of the Second Affiliated Hospital of Zhejiang University in October 2004 with right upper quadrant pain and weight loss.
+She was a hepatitis B virus carrier.
+Her α-fetoprotein level was 1185.3 ng/mL.
+Ultrasonography and computed tomography (CT) revealed a 10-cm mass in the posterior segments of the right liver lobe.
+A 1.5-cm mass was also found in the left lateral segment.
+These clinical signs indicated that the patient had inoperable HCC and Child-Pugh class A cirrhosis.
+TACE was offered to the patient.
+Angiogram demonstrated no obvious hepatic arterio-venous shunt, but multiple smaller masses in both lobes of the liver.
+An emulsion of oxaliplatin, pirarubicin, hydroxycamptothecin and lipiodol were prepared, 35 mL and 3 mL of the mixture were administered intra-arterially to the right and left hepatic artery, respectively.
+The patient experienced right upper quadrant pain after TACE and had an uneventful recovery.
+One month later, a second TACE procedure was performed via the right hepatic artery and 40 mL of the mixture was administered.
+On the next day, she experienced sudden acute dyspnoea and the peripheral oxygen saturation decreased to 90%.
+The chest X-ray showed some increased reticular shadows in the left lung, especially in the lower zones, and a chest CT scan revealed multiple iodized oil-like high-density materials in parenchyma of the lung (Figure ​1).
+After 10 mg dexamethasone i.v. and other supportive therapies were administered, the respiratory symptom was attenuated.
+Two days later, the patient suffered from a serious headache and transient consciousness loss, accompanying nausea and vomiting followed by confusion, lower extremity weakness.
+Non-contrast enhanced CT scanning showed multiple disseminated hyper-intense lesions in the brain, consistent with deposition of iodized oil (Figure ​2).
+One week later, her respiratory and neurologic symptoms disappeared completely, and she was discharged.
+The patient also consequently completed the other three TACE procedures, during which no similar symptoms occurred.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 71-year-old woman with known diastolic congestive heart failure (CHF) presented to the ER with exacerbation of CHF and a decreased level of consciousness.
+Brachial blood pressure (BP) was measured at 55/40 mmHg.
+The patient had four recent admissions with exacerbation of CHF.
+Her medical history was also significant for autoimmune hepatitis, but preserved liver function; esophageal varices with a bleeding episode; and long-term corticosteroid therapy complicated by adrenal insufficiency, type 2 diabetes mellitus and osteoporosis.
+Recent echocardiography had revealed moderate concentric left ventricular hypertrophy with diastolic dysfunction, and mild to moderate mitral regurgitation.
+Cardiac catheterization in a recent admission demonstrated 50% stenosis in the second diagonal artery, with mild diffuse disease in the other coronary arteries.
+Right ventricular endomyocardial biopsy had ruled out myocarditis and infiltrative cardiomyopathies, but healing ischemic microinfarcts with atheroemboli were observed.
+Previous BP values were also low; systolic BP was between 60 mmHg and 65 mmHg, and diastolic BP was between 40 mmHg and 45 mmHg.
+Following intubation, dopamine was started for hypotension management and was later replaced with noradrenaline.
+The patient developed atrial flutter but successfully converted to sinus rhythm with two direct current electric shocks.
+Cardiology consultation resulted in admission to the coronary care unit (CCU).
+On admission to the CCU, BP was measured at 56/36 mmHg in the left arm but was not detectable in the right arm.
+An arterial line was inserted via the femoral artery, and BP was measured at 191/92 mmHg.
+BP values were consistently much higher through the femoral arterial line than the cuff on the arms, and was higher in the left arm than in the right arm.
+For instance, on the first day post-CCU admission, BP at one point was measured at 170/80 mmHg through the arterial line, while cuff readings on the arms were 83/74 mmHg on the left and 60/39 mmHg on the right arm.
+To investigate the inconsistency between brachial and femoral BP values, a computed tomography (CT) scan of the thorax was obtained using 1.25 mm slices, both before and after intravenous contrast injection with sagittal and coronal planar reformatting of maximum-intensity projection images.
+Analysis of the initial unenhanced CT images showed densely calcified plaque or thrombus at the origins of both subclavian arteries and the right common carotid artery.
+The CT angiogram showed absence of flow in the right subclavian artery, a very tight stenosis at the origin of the left subclavian artery and a tight stenosis at the origin of the right common carotid artery.
+Both vertebral arteries showed normal calibre and flow (Figure 1).
+Further management following the insertion of the femoral arterial line was based on femoral BP readings with diuretics and BP-lowering agents.
+The patient was eventually discharged in stable condition.
+She remained stable during the eight months between discharge and the time the present report was written, without further exacerbation of CHF or related ER visits.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A newborn boy of healthy nonconsanguineous parents was delivered at 37 weeks’ gestation by cesarean section.
+His mother (primipara, 32 years old) had been admitted to our hospital 2 weeks previously because of reduced fetal intrauterine movements and polyhydramnios.
+The child’s birthweight was 2,330 g (&lt;10th percentile), length 47 cm, and head circumference 33.2 cm (25th percentile).
+He had low-set ears and bilateral clubfoot.
+Apgar scores were 2, 6, and 7 at 1, 5, and 10 minutes.
+The child presented with severe hypotonia and generalized muscle weakness, requiring ventilatory assistance and total parenteral nutrition.
+Weaning failed because of inadequate pulmonary ventilation and respiratory acidosis.
+Hearing loss was detected by auditory evoked potentials, while cranial MRI showed mildly enlarged ventricles and liquor spaces.
+Two days after birth, the infant presented with severe abdominal distension with a hypoactive bowel.
+MRI revealed marked intestinal dilation without mechanical obstruction.
+Laboratory investigations showed hypoglycemia (27 mg/dL), hypomagnesemia (0.58 mmol/L), and hypokalemia (2.4 mmol/L).
+Blood lactate was normal (1.3 mmol/L, normal range 0.5–2.2 mmol/L) and liver enzymes were unremarkable.
+A skeletal muscle biopsy was performed and showed scattered, hypertrophic cytochrome c oxidase (COX)-deficient and succinate dehydrogenase–positive muscle fibers (figure), suggesting a mitochondrial disorder.
+Molecular genetic studies revealed marked mtDNA depletion in muscle (93% decrease as compared to age-matched controls), while a screen for mtDNA rearrangements within individual COX-positive and COX-deficient fibers4 was negative.
+We sequenced the entire coding region and intron-exon boundaries of the POLG1 gene, identifying two reported heterozygous missense mutations in compound c.679C&gt;T predicting p.R227W and c.2542G&gt;A predicting p.G848S.
+Sequencing of parental samples confirmed recessive inheritance.
+The infant died at 20 days of respiratory failure.
+At autopsy, the brain did not show remarkable changes on gross examination.
+Histology was not informative due to poor preservation of tissue; there was no evidence of neuronal damage in the spinal cord.
+The liver showed diffuse cholestasis, consistent with total parenteral nutrition; hepatocyte steatosis, necrosis, or liver fibrosis were not observed.
+The testicles were undescended, while remaining visceral organs were normal except for a marked dilation and thinning of the bowel wall.
+Despite normal histology, analysis of stomach, ileum, and colon homogenates revealed severe mtDNA depletion (up to 94% decrease; table e-1 on the Neurology® Web site at www.neurology.org).
+Laser capture microdissection analysis5 revealed that the mtDNA depletion was confined to the muscularis propria, being most prominent in its external layer (figure).
+Ganglion cells from the myenteric plexus showed milder mtDNA depletion, restricted to the small intestine (figure).
+There was no mtDNA depletion in liver (not shown).
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 46-year-old woman presented with severe acute pain in the right iliac fossa and periumbilical region.
+Ultrasound and a computed tomography scan revealed a mucocele in the vermiform appendix, with a well defined lesion located at the mid zone of the appendix.
+The patient underwent right hemicolectomy, and her postoperative clinical course was uneventful.
+Gross examination of the surgical specimen showed an enlarged appendix, which was filled with thick mucinous material.
+A distinct lesion which involved the appendiceal wall, and measured 1.5 cm maximally, was identified in the mid-portion of the appendix.
+There was no evidence of perforation, extravasation of mucin into the periappendiceal tissue, or pseudomyxoma peritonei during surgery.
+Histopathological examination showed combined GCC and MCA of the vermiform appendix (Figure ​1A).
+The appendiceal lumen was dilated and lined by mucin-containing columnar epithelial cells (Figure 1B).
+There was no significant cytologic atypia, and no mitotic figures were identified.
+Focal papillary configurations of the lining epithelium, and mild epithelial pseudostratification were present.
+In addition, the appendiceal wall was infiltrated by glandular structures of various sizes which were arranged in nests and tubules.
+These glandular structures comprised 2 distinct types of cells: (1) small to intermediate sized monotonous neuroendocrine cells with a small amount of finely granular eosinophilic cytoplasm, and mild cytonuclear atypia (Figure ​(Figure1C);1C); (2) mucin-filled intermediate sized cells (goblet cells), with peripherally located small, crescent-like hyperchromatic nuclei, and indistinct nucleoli (Figure ​(Figure1D).1D).
+Scattered infiltrating single goblet neoplastic cells were focally present.
+As previously described[1] the tumor nests appeared to arise from the basiglandular region of the intestinal crypts in close proximity to the MCA (Figure ​(Figure1E).1E).
+There was no lymphovascular invasion, although perineural and intraneural invasion was present.
+The tumor infiltrated the full thickness of the appendiceal wall and extended to the mesoappendix.
+Ten lymph nodes were histologically identified, of which all were negative for malignancy.
+Immunohistochemically (Table ​1), the tumor cells of the GCC were positive for chromogranin, synaptophysin, and serotonin, which are neuroendocrine markers.
+Diffuse staining for cytokeratin (CK) 20 (Figure ​2), CK19, and CD99 was also present.
+The Ki67 proliferating index revealed nuclear staining in approximately 15% of the tumor cells.
+There was no staining for CK7.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 60-year-old man who underwent colonoscopy was found to have a 2 cm sessile polyp that was located 10 cm from the anal verge and successfully removed.
+The polyp was a tubulovillous adenoma with focal high-grade dysplasia.
+A flexible sigmoidoscopy performed three months later, as well as a repeat colonoscopy one year after the initial colonoscopy, were both negative for recurrence.
+A colonoscopy performed three years after the initial colonoscopy revealed a sessile polyp, 3 cm in size, at 10 cm from the anal verge.
+Biopsies were taken and reported to be fragments of a villous adenoma with low-grade dysplasia.
+Due to the previous high-grade dysplasia, relatively rapid recurrence and concern that a cancer may have been missed by sampling error, a pelvic magnetic resonance imaging (MRI) scan and an endoscopic ultrasound (EUS) were performed before definitive excision.
+The MRI revealed an invasive rectal mass involving the muscularis propria but without breach of the adventitia, consistent with a T2 rectal carcinoma (Figure 1).
+No pelvic lymphadenopathy was detected.
+The EUS revealed a rectal mass involving the mucosa and submucosa, with no involvement of the muscularis propria (Figure 2).
+The results of the MRI and EUS, as well as the surgical versus endoscopic resection treatment options, were discussed with the patient, who opted for a surgical resection.
+The patient underwent a low anterior resection and end-to-end anastomosis with loop ileostomy.
+Pathology review of the resected rectosigmoid revealed a villous adenoma with low-grade dyplasia.
+There was no evidence of muscularis propria invasion, and a total of five pericolic and two mesorectal lymph nodes were excised and deemed benign.
+The patient underwent ileostomy reversal five months later.
+He remains asymptomatic with no recurrence of tumours.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 72-year-old woman underwent RF ablation for the treatment of a metachronous solitary liver metastasis from rectal adenocarcinoma, which had been treated 18 mo before with preoperative chemoradiotherapy and anterior resection.
+The lesion was located in segment VIII.
+The procedure went well and the patient was initially haemodynamically stable.
+One hour later her condition suddenly worsened.
+She was clinically dizzy and had fatigue and pallor.
+We detected hypotension and tachycardia.
+Emergency blood tests showed a haemoglobin level of &lt; 7 g/dL and markedly elevated transaminase levels.
+A computed tomography examination revealed an accumulation of intraperitoneal fluid in the pelvis and two liver haematomas.
+The images showed two liver lacerations, one following the path of the needle (Figure ​(Figure1A1A-​-C)C) and another, unexplained laceration leading away from the first (Figure ​(Figure2).2).
+The patient had no serious coughing or hiccupping after the RF treatment, or any other complications that might have caused increased abdominal pressure and tumour rupture.
+Subsequently, the patient received a blood transfusion and close monitoring.
+She was haemodynamically stable after the second blood transfusion and completely recovered 24 h later.
+The patient remained in bed for 1 wk.
+No surgical intervention was required.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 70-year-old man was referred to our hospital for gastric cancer that was detected during screening by esophagogastroduodenoscopy (EGD).
+No significant medical history was identified, except dysuria caused by bladder contraction.
+Initial laboratory data showed a serum level of AFP of 32.3 ng/mL (normal range: 0-15 ng/mL), but no other abnormality, which included other tumor markers, such as, carcinoembryonic antigen (CEA) and carbohydrate antigen 19-9 (CA19-9).
+EGD revealed a 5-cm ulcerofungating mass that was comprised of three septate ulcers in the greater curvature of the gastric antrum.
+A pathological examination of endoscopic biopsy tissues confirmed the presence of moderately differentiated tubular adenocarcinoma.
+Subsequent abdominopelvic computed tomography visualized a gastric mass with deep ulceration in the gastric antrum with perigastric lymph node enlargement.
+No metastatic lesions were observed in the liver, lung or peritoneum, and chest radiography showed no significant findings.
+Radical subtotal gastrectomy with D2 lymph node dissection and Billroth II gastrojejunostomy were performed.
+Grossly, the resected specimen contained double lesions: the first was a 5.8 cm × 3.2 cm ulcerofungating mass in the antrum, with extensive hemorrhage and light gray fibrosis; and the second was a nearby 2.5 cm × 2.0 cm ulcerative lesion (Figure ​1).
+Microscopically, massive numbers of pleomorphic, bizarre tumor cells with hemorrhage (syncytiotrophoblasts and cytotrophoblasts) were observed in the first lesion.
+Hematoxylin and eosin (HE)-stained tissues revealed a bubbly purple cytoplasm and giant nuclei at a magnification of 40 × (Figure ​2A) and 100 × (Figure ​2B).
+The tumor involved the proper muscle layer (T2a) and metastasis was found in four of 56 regional lymph nodes (N1).
+Immunohistochemical staining showed positive immunoreactivity for β-human chorionic gonadotropin (HCG) (Figure ​3A) and focal positivity for AFP (Figure ​3B).
+These findings confirmed the presence of gastric choriocarcinoma that contained small foci of an AFP-producing adenocarcinoma.
+The second lesion was moderately differentiated tubular adenocarcinoma, which extended to the submucosal layer (T1b).
+It was close to, but distinct from the first lesion, which was negative by immunohistochemical staining for β-HCG and AFP.
+The patient had an uneventful postoperative course and was discharged on postoperative day 9.
+Two weeks later, his HCG level was 176 mIU/mL (normal range: 0-10 mIU/mL) and his AFP level was 10.0 ng/mL.
+Six cycles of adjuvant chemotherapy with capecitabine (Xeloda; Hoffmann-La Roche Inc., Nutley, NJ, USA) was started at 2500 mg/m2 per day for 14 d/cycle.
+After two cycles, his β-HCG level had declined to &lt; 3 mIU/mL, and has since remained at this level.
+No recurrence or distant metastasis had occurred at his 4-year postoperative follow-up.
+</t>
   </si>
   <si>
     <t>An 81-year-old female with hypertension and gout was admitted to Taichung Veterans General Hospital due to abdominal pain and hematemesis.
@@ -50,7 +428,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,6 +439,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -92,14 +476,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -107,10 +485,13 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -414,28 +795,111 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="76.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25" customFormat="1" s="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="2619" customFormat="1" s="3">
-      <c r="A2" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+      <c r="A3" s="3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+      <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+      <c r="A15" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+      <c r="A16" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+      <c r="A17" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+      <c r="A18" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+      <c r="A19" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="2863.5" customFormat="1" s="1">
+      <c r="A20" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>